<commit_message>
05/01/26 - adding Sainsbury's shopping and 200GB SIM card purchase
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztofzdanowicz/Documents/Development/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B690D68-C7E1-5A46-B502-067000A29F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FA9B7E-D7F3-3D49-8B7B-DD2DEA95146F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="1" xr2:uid="{DE091AD9-5213-A147-A202-F086AB57A082}"/>
   </bookViews>
@@ -47,7 +47,7 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    initial purchases such as duvet, pillow, blanket, pan, pot, kettle, plates, toilet brush, vacuum cleaner etc. + Ubers from the airport to the flat with the luggage</t>
+    initial purchases such as duvet, pillow, blanket, pan, pot, kettle, plates, toilet brush, vacuum cleaner etc. + Ubers from the airport to the flat with the luggage + large mobile data SIM card</t>
       </text>
     </comment>
   </commentList>
@@ -111,9 +111,6 @@
     <t>Utilities</t>
   </si>
   <si>
-    <t>Total + Utilities + Rent</t>
-  </si>
-  <si>
     <t>February</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>April</t>
+  </si>
+  <si>
+    <t>Total + Utilities</t>
   </si>
 </sst>
 </file>
@@ -199,11 +199,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,7 +546,7 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="O2" dT="2026-01-04T20:16:50.79" personId="{1AF904E1-D543-E942-A7CB-C243F43C4213}" id="{91C9C1EA-A455-B54D-893A-C6D10036B888}">
-    <text>initial purchases such as duvet, pillow, blanket, pan, pot, kettle, plates, toilet brush, vacuum cleaner etc. + Ubers from the airport to the flat with the luggage</text>
+    <text>initial purchases such as duvet, pillow, blanket, pan, pot, kettle, plates, toilet brush, vacuum cleaner etc. + Ubers from the airport to the flat with the luggage + large mobile data SIM card</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -570,7 +570,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -630,7 +630,7 @@
         <v>17</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>11</v>
@@ -639,10 +639,10 @@
         <v>12</v>
       </c>
       <c r="Q1" s="3"/>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="6"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -664,7 +664,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="J2" s="4">
         <v>27</v>
@@ -672,7 +672,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4">
         <f>H2+I2+J2+K2</f>
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="M2" s="4">
         <f>C2+D2+E2+F2+G2</f>
@@ -680,21 +680,21 @@
       </c>
       <c r="N2" s="4">
         <f>B2+L2+M2</f>
-        <v>2021</v>
+        <v>2030</v>
       </c>
       <c r="O2" s="4">
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>14</v>
       </c>
       <c r="Q2" s="5"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4">
         <v>1800</v>
@@ -729,12 +729,12 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>1800</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4">
         <v>1800</v>
@@ -1002,202 +1002,202 @@
       <c r="S14" s="5"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-      <c r="L25" s="7"/>
-      <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="7"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
6th Jan 2026 - Sainsbury's
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztofzdanowicz/Documents/Development/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FA9B7E-D7F3-3D49-8B7B-DD2DEA95146F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD77369D-6B19-5343-BC3C-823A1745E9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="1" xr2:uid="{DE091AD9-5213-A147-A202-F086AB57A082}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,7 +664,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="J2" s="4">
         <v>27</v>
@@ -672,7 +672,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4">
         <f>H2+I2+J2+K2</f>
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="M2" s="4">
         <f>C2+D2+E2+F2+G2</f>
@@ -680,7 +680,7 @@
       </c>
       <c r="N2" s="4">
         <f>B2+L2+M2</f>
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="O2" s="4">
         <v>340</v>

</xml_diff>

<commit_message>
7th Jan 2026 - Tesco's
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztofzdanowicz/Documents/Development/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD77369D-6B19-5343-BC3C-823A1745E9FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DEE4E21-CA00-374A-AE25-F457430F74EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="1" xr2:uid="{DE091AD9-5213-A147-A202-F086AB57A082}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,7 +664,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="J2" s="4">
         <v>27</v>
@@ -672,7 +672,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4">
         <f>H2+I2+J2+K2</f>
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="M2" s="4">
         <f>C2+D2+E2+F2+G2</f>
@@ -680,7 +680,7 @@
       </c>
       <c r="N2" s="4">
         <f>B2+L2+M2</f>
-        <v>2040</v>
+        <v>2055</v>
       </c>
       <c r="O2" s="4">
         <v>340</v>

</xml_diff>

<commit_message>
10th Jan 2026: Sainsbury's
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krzysztofzdanowicz/Documents/Development/budget/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A1F1BE-C338-8F47-A515-86E8B0770C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2901619C-78C7-7F4D-A6D3-235DF6DD6213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="1" xr2:uid="{DE091AD9-5213-A147-A202-F086AB57A082}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -664,7 +664,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="J2" s="4">
         <v>32</v>
@@ -672,7 +672,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4">
         <f>H2+I2+J2+K2</f>
-        <v>131</v>
+        <v>166</v>
       </c>
       <c r="M2" s="4">
         <f>C2+D2+E2+F2+G2</f>
@@ -680,10 +680,10 @@
       </c>
       <c r="N2" s="4">
         <f>B2+L2+M2</f>
-        <v>2060</v>
+        <v>2095</v>
       </c>
       <c r="O2" s="4">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>14</v>

</xml_diff>